<commit_message>
Fix some bugs and add post questions
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Tabelle3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Tabelle4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
   <si>
     <t xml:space="preserve">M = Meine Anwendung</t>
   </si>
@@ -367,6 +368,12 @@
   </si>
   <si>
     <t xml:space="preserve">27:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haus am See</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haus am see</t>
   </si>
 </sst>
 </file>
@@ -499,7 +506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,23 +607,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -727,7 +718,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1168,7 +1159,7 @@
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1337,23 +1328,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="7" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,18 +1354,15 @@
         <v>4</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="16" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1386,19 +1373,16 @@
       <c r="B2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="17" t="n">
-        <v>3</v>
+      <c r="C2" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="19" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1410,21 +1394,18 @@
         <v>80</v>
       </c>
       <c r="C3" s="21" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D3" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="21" t="n">
         <v>0</v>
       </c>
+      <c r="E3" s="22" t="n">
+        <v>0.331944444444444</v>
+      </c>
       <c r="F3" s="22" t="n">
-        <v>0.331944444444444</v>
-      </c>
-      <c r="G3" s="22" t="n">
         <v>0.654166666666667</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -1433,19 +1414,16 @@
       <c r="B4" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="25" t="n">
-        <v>3</v>
+      <c r="C4" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="19" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1456,22 +1434,19 @@
       <c r="B5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>13</v>
+      <c r="D5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="n">
@@ -1480,19 +1455,16 @@
       <c r="B6" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="25" t="n">
-        <v>3</v>
+      <c r="C6" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="19" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1503,19 +1475,16 @@
       <c r="B7" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>13</v>
+      <c r="D7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="22" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1526,19 +1495,16 @@
       <c r="B8" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>28</v>
+      <c r="C8" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="19" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1549,19 +1515,16 @@
       <c r="B9" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>13</v>
+      <c r="D9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1572,19 +1535,16 @@
       <c r="B10" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>28</v>
+      <c r="C10" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="19" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1595,19 +1555,16 @@
       <c r="B11" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>13</v>
+      <c r="D11" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>101</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" s="22" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1618,19 +1575,16 @@
       <c r="B12" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>32</v>
+      <c r="C12" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="19" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1641,19 +1595,16 @@
       <c r="B13" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>13</v>
+      <c r="D13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>105</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1664,19 +1615,16 @@
       <c r="B14" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>32</v>
+      <c r="C14" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="19" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1687,19 +1635,16 @@
       <c r="B15" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="27" t="s">
-        <v>13</v>
+      <c r="D15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>109</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="22" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1710,19 +1655,16 @@
       <c r="B16" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>32</v>
+      <c r="C16" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>13</v>
+        <v>13</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="19" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1733,19 +1675,16 @@
       <c r="B17" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="27" t="s">
-        <v>13</v>
+      <c r="D17" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" s="22" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1758,4 +1697,91 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="A1:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update analysis and also analyse pretask
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,16 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
-  <si>
-    <t xml:space="preserve">M = Meine Anwendung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO : Task Success Percentage direkt in R schneller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO 2 time in time start und time end und dann in r in sec rechnen?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="113">
   <si>
     <t xml:space="preserve">Proband</t>
   </si>
@@ -107,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">M + Erlangen + B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
@@ -717,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A1:F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,61 +719,53 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
-      <c r="I2" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>267</v>
@@ -793,13 +773,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>3</v>
@@ -808,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>464</v>
@@ -817,22 +797,22 @@
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6" s="3" t="n">
         <v>337</v>
@@ -840,22 +820,22 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>97</v>
@@ -863,22 +843,22 @@
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>402</v>
@@ -886,22 +866,22 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>277</v>
@@ -909,22 +889,22 @@
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>309</v>
@@ -932,22 +912,22 @@
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>189</v>
@@ -955,22 +935,22 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="9" t="n">
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>216</v>
@@ -978,22 +958,22 @@
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="9" t="n">
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>46</v>
@@ -1001,22 +981,22 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>124</v>
@@ -1024,22 +1004,22 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G15" s="3" t="n">
         <v>86</v>
@@ -1047,22 +1027,22 @@
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>112</v>
@@ -1070,22 +1050,22 @@
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>64</v>
@@ -1093,45 +1073,45 @@
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>145</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C19" s="9" t="n">
+        <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>79</v>
@@ -1159,7 +1139,7 @@
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:F17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1171,67 +1151,67 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -1241,7 +1221,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1251,62 +1231,62 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1330,8 +1310,8 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1348,22 +1328,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,19 +1351,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C3" s="21" t="n">
         <v>3</v>
@@ -1412,19 +1392,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,19 +1412,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H5" s="23"/>
     </row>
@@ -1453,19 +1433,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,19 +1453,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,19 +1473,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,19 +1493,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,19 +1513,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,19 +1533,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,19 +1553,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,19 +1573,19 @@
         <v>2</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,19 +1593,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,19 +1613,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,19 +1633,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,19 +1653,19 @@
         <v>2</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +1687,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="A1:F17"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="A1:A2 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1717,62 +1697,62 @@
   <sheetData>
     <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the last participants and reorganize results
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael_M\Documents\GitHub\BA_Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF5213E-C4AB-41F7-926D-4A91DE5CCACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4355E7-6612-4189-9C74-FEB4289C89B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="0" windowWidth="12540" windowHeight="10200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studie" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="255">
   <si>
     <t>Proband</t>
   </si>
@@ -399,30 +399,6 @@
     <t>53:37</t>
   </si>
   <si>
-    <t>1:05:34</t>
-  </si>
-  <si>
-    <t>1:06:15</t>
-  </si>
-  <si>
-    <t>1:18:19</t>
-  </si>
-  <si>
-    <t>1:18:49</t>
-  </si>
-  <si>
-    <t>TODO in minuten umrechnen?</t>
-  </si>
-  <si>
-    <t>1:30:20</t>
-  </si>
-  <si>
-    <t>1:31:24</t>
-  </si>
-  <si>
-    <t>1:34:35</t>
-  </si>
-  <si>
     <t>2:12</t>
   </si>
   <si>
@@ -528,9 +504,6 @@
     <t>58:12</t>
   </si>
   <si>
-    <t>1:04:39</t>
-  </si>
-  <si>
     <t>2:10</t>
   </si>
   <si>
@@ -615,15 +588,6 @@
     <t>55:53</t>
   </si>
   <si>
-    <t>1:00:02</t>
-  </si>
-  <si>
-    <t>1:00:43</t>
-  </si>
-  <si>
-    <t>1:02:16</t>
-  </si>
-  <si>
     <t>03:04</t>
   </si>
   <si>
@@ -670,6 +634,162 @@
   </si>
   <si>
     <t>45:40</t>
+  </si>
+  <si>
+    <t>5:43</t>
+  </si>
+  <si>
+    <t>6:56</t>
+  </si>
+  <si>
+    <t>14:41</t>
+  </si>
+  <si>
+    <t>16:07</t>
+  </si>
+  <si>
+    <t>22:23</t>
+  </si>
+  <si>
+    <t>25:48</t>
+  </si>
+  <si>
+    <t>27:21</t>
+  </si>
+  <si>
+    <t>28:17</t>
+  </si>
+  <si>
+    <t>29:22</t>
+  </si>
+  <si>
+    <t>30:14</t>
+  </si>
+  <si>
+    <t>32:45</t>
+  </si>
+  <si>
+    <t>33:30</t>
+  </si>
+  <si>
+    <t>40:58</t>
+  </si>
+  <si>
+    <t>2:06</t>
+  </si>
+  <si>
+    <t>4:08</t>
+  </si>
+  <si>
+    <t>5:33</t>
+  </si>
+  <si>
+    <t>6:52</t>
+  </si>
+  <si>
+    <t>7:41</t>
+  </si>
+  <si>
+    <t>12:09</t>
+  </si>
+  <si>
+    <t>16:03</t>
+  </si>
+  <si>
+    <t>19:58</t>
+  </si>
+  <si>
+    <t>23:09</t>
+  </si>
+  <si>
+    <t>33:54</t>
+  </si>
+  <si>
+    <t>35:32</t>
+  </si>
+  <si>
+    <t>36:01</t>
+  </si>
+  <si>
+    <t>38:27</t>
+  </si>
+  <si>
+    <t>40:18</t>
+  </si>
+  <si>
+    <t>42:28</t>
+  </si>
+  <si>
+    <t>3:22</t>
+  </si>
+  <si>
+    <t>9:23</t>
+  </si>
+  <si>
+    <t>11:01</t>
+  </si>
+  <si>
+    <t>16:17</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>22:27</t>
+  </si>
+  <si>
+    <t>32:06</t>
+  </si>
+  <si>
+    <t>34:32</t>
+  </si>
+  <si>
+    <t>35:31</t>
+  </si>
+  <si>
+    <t>38:26</t>
+  </si>
+  <si>
+    <t>40:29</t>
+  </si>
+  <si>
+    <t>39:37</t>
+  </si>
+  <si>
+    <t>42:50</t>
+  </si>
+  <si>
+    <t>60:43</t>
+  </si>
+  <si>
+    <t>62:16</t>
+  </si>
+  <si>
+    <t>60:02</t>
+  </si>
+  <si>
+    <t>64:39</t>
+  </si>
+  <si>
+    <t>94:35</t>
+  </si>
+  <si>
+    <t>90:20</t>
+  </si>
+  <si>
+    <t>91:24</t>
+  </si>
+  <si>
+    <t>78:49</t>
+  </si>
+  <si>
+    <t>78:19</t>
+  </si>
+  <si>
+    <t>66:15</t>
+  </si>
+  <si>
+    <t>65:34</t>
   </si>
 </sst>
 </file>
@@ -1426,9 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1692,7 +1810,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>3</v>
@@ -1772,7 +1890,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>3</v>
@@ -1952,7 +2070,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>4</v>
@@ -2084,7 +2202,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>4</v>
       </c>
@@ -2104,7 +2222,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>5</v>
       </c>
@@ -2124,7 +2242,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>5</v>
       </c>
@@ -2132,7 +2250,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>3</v>
@@ -2144,7 +2262,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>5</v>
       </c>
@@ -2164,7 +2282,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>5</v>
       </c>
@@ -2184,7 +2302,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>5</v>
       </c>
@@ -2201,13 +2319,10 @@
         <v>123</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="H38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>5</v>
       </c>
@@ -2221,13 +2336,13 @@
         <v>3</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>125</v>
+        <v>253</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>5</v>
       </c>
@@ -2241,13 +2356,13 @@
         <v>3</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>127</v>
+        <v>251</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="11">
         <v>5</v>
       </c>
@@ -2261,13 +2376,13 @@
         <v>3</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>6</v>
       </c>
@@ -2275,19 +2390,19 @@
         <v>29</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
         <v>6</v>
       </c>
@@ -2301,13 +2416,13 @@
         <v>3</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>6</v>
       </c>
@@ -2321,13 +2436,13 @@
         <v>3</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>6</v>
       </c>
@@ -2341,13 +2456,13 @@
         <v>3</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>6</v>
       </c>
@@ -2355,19 +2470,19 @@
         <v>26</v>
       </c>
       <c r="C46" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="F46" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>6</v>
       </c>
@@ -2381,13 +2496,13 @@
         <v>3</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>6</v>
       </c>
@@ -2401,10 +2516,10 @@
         <v>3</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2421,10 +2536,10 @@
         <v>3</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2441,7 +2556,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F50" s="13" t="s">
         <v>116</v>
@@ -2461,10 +2576,10 @@
         <v>4</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2475,16 +2590,16 @@
         <v>29</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2501,10 +2616,10 @@
         <v>3</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2521,10 +2636,10 @@
         <v>4</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2535,16 +2650,16 @@
         <v>16</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2561,10 +2676,10 @@
         <v>3</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2581,10 +2696,10 @@
         <v>3</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2601,10 +2716,10 @@
         <v>3</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2621,10 +2736,10 @@
         <v>3</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2641,10 +2756,10 @@
         <v>3</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2661,10 +2776,10 @@
         <v>3</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2681,10 +2796,10 @@
         <v>3</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2701,10 +2816,10 @@
         <v>3</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2721,10 +2836,10 @@
         <v>3</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -2741,10 +2856,10 @@
         <v>2</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>197</v>
+        <v>244</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>198</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -2855,7 +2970,7 @@
         <v>26</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D71" s="17" t="s">
         <v>3</v>
@@ -2875,7 +2990,7 @@
         <v>29</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>3</v>
@@ -2975,7 +3090,7 @@
         <v>26</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D77" s="17" t="s">
         <v>3</v>
@@ -3055,7 +3170,7 @@
         <v>29</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D81" s="17" t="s">
         <v>3</v>
@@ -3175,7 +3290,7 @@
         <v>29</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D87" s="17" t="s">
         <v>3</v>
@@ -3241,10 +3356,10 @@
         <v>3</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -3261,10 +3376,10 @@
         <v>4</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -3281,10 +3396,10 @@
         <v>3</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -3301,10 +3416,10 @@
         <v>3</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -3321,10 +3436,10 @@
         <v>3</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -3341,10 +3456,10 @@
         <v>3</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -3361,10 +3476,10 @@
         <v>3</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -3381,10 +3496,10 @@
         <v>4</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -3401,10 +3516,10 @@
         <v>3</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -3421,10 +3536,10 @@
         <v>3</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -3441,10 +3556,10 @@
         <v>3</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -3461,10 +3576,10 @@
         <v>1</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -3481,10 +3596,10 @@
         <v>1</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -3501,10 +3616,10 @@
         <v>1</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -3521,10 +3636,10 @@
         <v>3</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -3541,10 +3656,10 @@
         <v>1</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -3554,12 +3669,18 @@
       <c r="B106" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C106" s="18"/>
+      <c r="C106" s="18">
+        <v>4</v>
+      </c>
       <c r="D106" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E106" s="13"/>
-      <c r="F106" s="13"/>
+      <c r="E106" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F106" s="13" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="11">
@@ -3568,12 +3689,18 @@
       <c r="B107" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C107" s="18"/>
-      <c r="D107" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E107" s="13"/>
-      <c r="F107" s="13"/>
+      <c r="C107" s="18">
+        <v>1</v>
+      </c>
+      <c r="D107" s="17">
+        <v>1</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F107" s="13" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="11">
@@ -3582,12 +3709,18 @@
       <c r="B108" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C108" s="18"/>
+      <c r="C108" s="18">
+        <v>1</v>
+      </c>
       <c r="D108" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E108" s="13"/>
-      <c r="F108" s="13"/>
+      <c r="E108" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F108" s="13" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="11">
@@ -3596,12 +3729,18 @@
       <c r="B109" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C109" s="18"/>
-      <c r="D109" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E109" s="13"/>
-      <c r="F109" s="13"/>
+      <c r="C109" s="18">
+        <v>0</v>
+      </c>
+      <c r="D109" s="17">
+        <v>2</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F109" s="13" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="11">
@@ -3610,12 +3749,18 @@
       <c r="B110" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C110" s="18"/>
+      <c r="C110" s="18">
+        <v>8</v>
+      </c>
       <c r="D110" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
+      <c r="E110" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F110" s="13" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="11">
@@ -3624,12 +3769,18 @@
       <c r="B111" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C111" s="18"/>
+      <c r="C111" s="18">
+        <v>2</v>
+      </c>
       <c r="D111" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
+      <c r="E111" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F111" s="13" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="11">
@@ -3638,12 +3789,18 @@
       <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="18"/>
+      <c r="C112" s="18">
+        <v>3</v>
+      </c>
       <c r="D112" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
+      <c r="E112" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F112" s="13" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="11">
@@ -3652,12 +3809,18 @@
       <c r="B113" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C113" s="18"/>
-      <c r="D113" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
+      <c r="C113" s="18">
+        <v>0</v>
+      </c>
+      <c r="D113" s="17">
+        <v>1</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F113" s="13" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="11">
@@ -3666,12 +3829,18 @@
       <c r="B114" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C114" s="18"/>
+      <c r="C114" s="18">
+        <v>2</v>
+      </c>
       <c r="D114" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E114" s="13"/>
-      <c r="F114" s="13"/>
+      <c r="E114" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F114" s="13" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="11">
@@ -3680,12 +3849,18 @@
       <c r="B115" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C115" s="18"/>
+      <c r="C115" s="18">
+        <v>1</v>
+      </c>
       <c r="D115" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E115" s="13"/>
-      <c r="F115" s="13"/>
+      <c r="E115" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F115" s="13" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="11">
@@ -3694,12 +3869,18 @@
       <c r="B116" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C116" s="18"/>
+      <c r="C116" s="18">
+        <v>1</v>
+      </c>
       <c r="D116" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
+      <c r="E116" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="F116" s="13" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="11">
@@ -3708,12 +3889,18 @@
       <c r="B117" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C117" s="18"/>
+      <c r="C117" s="18">
+        <v>2</v>
+      </c>
       <c r="D117" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
+      <c r="E117" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F117" s="13" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="11">
@@ -3722,12 +3909,18 @@
       <c r="B118" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C118" s="18"/>
+      <c r="C118" s="18">
+        <v>1</v>
+      </c>
       <c r="D118" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
+      <c r="E118" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="F118" s="13" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="11">
@@ -3736,12 +3929,18 @@
       <c r="B119" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C119" s="18"/>
+      <c r="C119" s="18">
+        <v>1</v>
+      </c>
       <c r="D119" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
+      <c r="E119" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F119" s="13" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="11">
@@ -3750,12 +3949,18 @@
       <c r="B120" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C120" s="18"/>
+      <c r="C120" s="18">
+        <v>9</v>
+      </c>
       <c r="D120" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
+      <c r="E120" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F120" s="13" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="11">
@@ -3764,12 +3969,18 @@
       <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="18"/>
+      <c r="C121" s="18">
+        <v>3</v>
+      </c>
       <c r="D121" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E121" s="13"/>
-      <c r="F121" s="13"/>
+      <c r="E121" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="F121" s="13" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="11">
@@ -3778,12 +3989,18 @@
       <c r="B122" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C122" s="18"/>
-      <c r="D122" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
+      <c r="C122" s="18">
+        <v>1</v>
+      </c>
+      <c r="D122" s="17">
+        <v>1</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F122" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="11">
@@ -3792,12 +4009,18 @@
       <c r="B123" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C123" s="18"/>
+      <c r="C123" s="18">
+        <v>1</v>
+      </c>
       <c r="D123" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
+      <c r="E123" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="F123" s="13" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="11">
@@ -3806,12 +4029,18 @@
       <c r="B124" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C124" s="18"/>
-      <c r="D124" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
+      <c r="C124" s="18">
+        <v>1</v>
+      </c>
+      <c r="D124" s="17">
+        <v>2</v>
+      </c>
+      <c r="E124" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="F124" s="13" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="11">
@@ -3820,12 +4049,18 @@
       <c r="B125" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C125" s="18"/>
+      <c r="C125" s="18">
+        <v>4</v>
+      </c>
       <c r="D125" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
+      <c r="E125" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="F125" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="11">
@@ -3834,12 +4069,18 @@
       <c r="B126" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C126" s="18"/>
+      <c r="C126" s="18">
+        <v>6</v>
+      </c>
       <c r="D126" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
+      <c r="E126" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="F126" s="13" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="11">
@@ -3848,12 +4089,18 @@
       <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="18"/>
+      <c r="C127" s="18">
+        <v>1</v>
+      </c>
       <c r="D127" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
+      <c r="E127" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F127" s="13" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="11">
@@ -3862,12 +4109,18 @@
       <c r="B128" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C128" s="18"/>
+      <c r="C128" s="18">
+        <v>1</v>
+      </c>
       <c r="D128" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
+      <c r="E128" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="F128" s="13" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="11">
@@ -3876,12 +4129,18 @@
       <c r="B129" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C129" s="18"/>
+      <c r="C129" s="18">
+        <v>2</v>
+      </c>
       <c r="D129" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
+      <c r="E129" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F129" s="13" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>